<commit_message>
added SABR Hagan approximation formulas
</commit_message>
<xml_diff>
--- a/Distribution/Examples/ACQ.Stats.xlsx
+++ b/Distribution/Examples/ACQ.Stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C21053-B28D-45C5-8A19-4DB2DB4B3CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C286022C-4C69-459A-B943-C9AF50140F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
   <si>
     <t>date</t>
   </si>
@@ -2221,10 +2221,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30B9D5F-797C-49CC-9435-B3BF433B0ECB}">
-  <dimension ref="B1:L25"/>
+  <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2249,11 +2249,11 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">_xll.acq_min(H2:L18)</f>
-        <v>-0.98699999999999999</v>
+        <v>-0.94599999999999995</v>
       </c>
       <c r="D2" s="6">
         <f t="array" aca="1" ref="D2" ca="1">MIN(IF(ISNUMBER(H2:L18), H2:L18))</f>
-        <v>-0.98699999999999999</v>
+        <v>-0.94599999999999995</v>
       </c>
       <c r="E2">
         <f ca="1">C2-D2</f>
@@ -2261,23 +2261,23 @@
       </c>
       <c r="H2" s="5">
         <f ca="1">RANDBETWEEN(-1000,1000)/1000</f>
-        <v>-0.34200000000000003</v>
+        <v>0.33</v>
       </c>
       <c r="I2" s="5">
         <f t="shared" ref="I2:L18" ca="1" si="0">RANDBETWEEN(-1000,1000)/1000</f>
-        <v>-0.82699999999999996</v>
+        <v>0.439</v>
       </c>
       <c r="J2" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44700000000000001</v>
+        <v>-0.51400000000000001</v>
       </c>
       <c r="K2" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.98</v>
+        <v>0.57399999999999995</v>
       </c>
       <c r="L2" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81499999999999995</v>
+        <v>-0.14499999999999999</v>
       </c>
     </row>
     <row r="3" spans="2:12">
@@ -2286,7 +2286,7 @@
       </c>
       <c r="C3" s="6">
         <f ca="1">_xll.acq_absmin(H2:L18)</f>
-        <v>2.1999999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="D3" s="6">
         <f t="array" aca="1" ref="D3" ca="1">MIN(ABS(IF(ISNUMBER(H2:L18), H2:L18)))</f>
@@ -2294,27 +2294,27 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E11" ca="1" si="1">C3-D3</f>
-        <v>2.1999999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" ref="H3:H18" ca="1" si="2">RANDBETWEEN(-1000,1000)/1000</f>
-        <v>-2.1999999999999999E-2</v>
+        <v>-0.90100000000000002</v>
       </c>
       <c r="I3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.93700000000000006</v>
+        <v>-0.85399999999999998</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.223</v>
+        <v>-0.85</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47</v>
+        <v>-0.81299999999999994</v>
       </c>
       <c r="L3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.79800000000000004</v>
+        <v>0.10100000000000001</v>
       </c>
     </row>
     <row r="4" spans="2:12">
@@ -2323,11 +2323,11 @@
       </c>
       <c r="C4" s="6">
         <f ca="1">_xll.acq_max(H2:L18)</f>
-        <v>0.98</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="D4" s="6">
         <f t="array" aca="1" ref="D4" ca="1">MAX(IF(ISNUMBER(H2:L18), H2:L18))</f>
-        <v>0.98</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
@@ -2335,22 +2335,22 @@
       </c>
       <c r="H4" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.82699999999999996</v>
+        <v>-7.1999999999999995E-2</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.54200000000000004</v>
+        <v>0.05</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13800000000000001</v>
+        <v>-0.61799999999999999</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>56</v>
       </c>
       <c r="L4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.374</v>
+        <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="5" spans="2:12">
@@ -2359,11 +2359,11 @@
       </c>
       <c r="C5" s="6">
         <f ca="1">_xll.acq_absmax(H2:L18)</f>
-        <v>0.98699999999999999</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="D5" s="6">
         <f t="array" aca="1" ref="D5" ca="1">MAX(ABS(IF(ISNUMBER(H2:L18), H2:L18)))</f>
-        <v>0.98699999999999999</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
@@ -2371,22 +2371,22 @@
       </c>
       <c r="H5" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.875</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.80400000000000005</v>
+        <v>0.78600000000000003</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.14499999999999999</v>
+        <v>-0.86799999999999999</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.151</v>
+        <v>-0.13900000000000001</v>
       </c>
     </row>
     <row r="6" spans="2:12">
@@ -2395,11 +2395,11 @@
       </c>
       <c r="C6" s="6">
         <f ca="1">_xll.acq_sum(H2:L18)</f>
-        <v>-1.8860000000000006</v>
+        <v>-2.488</v>
       </c>
       <c r="D6" s="6">
         <f t="array" aca="1" ref="D6" ca="1">SUM(IF(ISNUMBER(H2:L18), H2:L18))</f>
-        <v>-1.885999999999999</v>
+        <v>-2.4879999999999995</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
@@ -2407,22 +2407,22 @@
       </c>
       <c r="H6" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>4.4999999999999998E-2</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.34100000000000003</v>
+        <v>0.45100000000000001</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.154</v>
+        <v>-4.3999999999999997E-2</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.82499999999999996</v>
+        <v>-0.27100000000000002</v>
       </c>
     </row>
     <row r="7" spans="2:12">
@@ -2431,7 +2431,7 @@
       </c>
       <c r="C7" s="6">
         <f ca="1">_xll.acq_count_unique(H2:L18)</f>
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D7" s="6">
         <f t="array" aca="1" ref="D7" ca="1">COUNT(H2:L18)</f>
@@ -2439,26 +2439,26 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.80400000000000005</v>
+        <v>-0.311</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>57</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.96499999999999997</v>
+        <v>-0.85799999999999998</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49</v>
+        <v>-0.62</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29599999999999999</v>
+        <v>0.54200000000000004</v>
       </c>
     </row>
     <row r="8" spans="2:12">
@@ -2467,11 +2467,11 @@
       </c>
       <c r="C8" s="6">
         <f ca="1">_xll.acq_mean(H2:L18)</f>
-        <v>-2.4815789473684218E-2</v>
+        <v>-3.2736842105263154E-2</v>
       </c>
       <c r="D8" s="6">
         <f t="array" aca="1" ref="D8" ca="1">AVERAGE(IF(ISNUMBER(H2:L18), H2:L18))</f>
-        <v>-2.4815789473684197E-2</v>
+        <v>-3.2736842105263154E-2</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
@@ -2479,23 +2479,23 @@
       </c>
       <c r="H8" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.38300000000000001</v>
+        <v>0.81499999999999995</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.95099999999999996</v>
+        <v>-0.69499999999999995</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.97599999999999998</v>
+        <v>-0.94599999999999995</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.27800000000000002</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.25600000000000001</v>
+        <v>-0.85899999999999999</v>
       </c>
     </row>
     <row r="9" spans="2:12">
@@ -2504,11 +2504,11 @@
       </c>
       <c r="C9" s="6">
         <f ca="1">_xll.acq_stdev(H2:L18)</f>
-        <v>0.61549051897439366</v>
+        <v>0.58206458675811457</v>
       </c>
       <c r="D9" s="6">
         <f t="array" aca="1" ref="D9" ca="1">_xlfn.STDEV.S(IF(ISNUMBER(H2:L18), H2:L18))</f>
-        <v>0.61549051897439355</v>
+        <v>0.58206458675811457</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
@@ -2516,22 +2516,22 @@
       </c>
       <c r="H9" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.626</v>
+        <v>0.04</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.92100000000000004</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>49</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.45400000000000001</v>
+        <v>0.626</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.51500000000000001</v>
+        <v>-0.50800000000000001</v>
       </c>
     </row>
     <row r="10" spans="2:12">
@@ -2540,11 +2540,11 @@
       </c>
       <c r="C10" s="6">
         <f ca="1">_xll.acq_sumofsquares(H2:L18)</f>
-        <v>28.458946000000001</v>
+        <v>25.491387999999997</v>
       </c>
       <c r="D10" s="6">
         <f t="array" aca="1" ref="D10" ca="1">SUM(IF(ISNUMBER(H2:L18), H2:L18^2))</f>
-        <v>28.458945999999994</v>
+        <v>25.491388000000001</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
@@ -2552,11 +2552,11 @@
       </c>
       <c r="H10" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.55200000000000005</v>
+        <v>0.41599999999999998</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.872</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="J10" s="5" t="e">
         <f>1/0</f>
@@ -2564,11 +2564,11 @@
       </c>
       <c r="K10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.753</v>
+        <v>-8.5000000000000006E-2</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23400000000000001</v>
+        <v>0.17199999999999999</v>
       </c>
     </row>
     <row r="11" spans="2:12">
@@ -2589,11 +2589,11 @@
       </c>
       <c r="H11" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.65200000000000002</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.68500000000000005</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="J11" s="5" t="e">
         <f>SQRT(-1)</f>
@@ -2601,163 +2601,163 @@
       </c>
       <c r="K11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13600000000000001</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.85199999999999998</v>
+        <v>0.97099999999999997</v>
       </c>
     </row>
     <row r="12" spans="2:12">
       <c r="H12" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.39</v>
+        <v>-0.81</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56499999999999995</v>
+        <v>0.59299999999999997</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>49</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.46700000000000003</v>
+        <v>-0.192</v>
       </c>
       <c r="L12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.186</v>
+        <v>0.29399999999999998</v>
       </c>
     </row>
     <row r="13" spans="2:12">
       <c r="H13" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.93700000000000006</v>
+        <v>-0.106</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31</v>
+        <v>-0.90900000000000003</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81100000000000005</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41099999999999998</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83799999999999997</v>
+        <v>0.88200000000000001</v>
       </c>
     </row>
     <row r="14" spans="2:12">
       <c r="H14" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.75800000000000001</v>
+        <v>0.22</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.88</v>
+        <v>0.60899999999999999</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.78600000000000003</v>
+        <v>0.42799999999999999</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33600000000000002</v>
+        <v>-0.1</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.20699999999999999</v>
+        <v>-5.2999999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="2:12">
       <c r="H15" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.153</v>
+        <v>-0.64300000000000002</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.95299999999999996</v>
+        <v>0.498</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.621</v>
+        <v>-0.128</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.1999999999999998E-2</v>
+        <v>0.96499999999999997</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.57899999999999996</v>
+        <v>-0.64100000000000001</v>
       </c>
     </row>
     <row r="16" spans="2:12">
       <c r="H16" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.24399999999999999</v>
+        <v>0.86299999999999999</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>9.9000000000000005E-2</v>
+        <v>-0.67</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.98699999999999999</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4999999999999998E-2</v>
+        <v>-0.52500000000000002</v>
       </c>
     </row>
     <row r="17" spans="2:12">
       <c r="H17" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89600000000000002</v>
+        <v>-0.76100000000000001</v>
       </c>
       <c r="I17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.35099999999999998</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="J17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94099999999999995</v>
+        <v>-0.85899999999999999</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.7000000000000002E-2</v>
+        <v>-0.26600000000000001</v>
       </c>
       <c r="L17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.78700000000000003</v>
+        <v>-0.35</v>
       </c>
     </row>
     <row r="18" spans="2:12">
       <c r="H18" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-8.5000000000000006E-2</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="I18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>9.9000000000000005E-2</v>
+        <v>-9.4E-2</v>
       </c>
       <c r="J18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44800000000000001</v>
+        <v>-0.65700000000000003</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.746</v>
+        <v>-0.71299999999999997</v>
       </c>
       <c r="L18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.53400000000000003</v>
+        <v>-0.63600000000000001</v>
       </c>
     </row>
     <row r="25" spans="2:12">
@@ -2766,7 +2766,25 @@
       </c>
       <c r="C25" t="str">
         <f ca="1">_xll.acq_join(H2:L18, "|")</f>
-        <v>-0.342|-0.022|-0.827|0.875|0.045|0.804|-0.383|-0.626|-0.552|0.652|0.39|0.937|-0.758|-0.153|-0.244|0.896|-0.085|-0.827|-0.937|-0.542|text|text|text3|-0.951|0.921|0.872|-0.685|0.565|0.31|-0.88|-0.953|text|0.351|0.099|0.447|-0.223|0.138|-0.804|-0.341|-0.965|-0.976|text|||text|0.811|-0.786|0.621|0.099|0.941|0.448|0.98|0.47|text2|-0.145|-0.154|0.49|-0.278|-0.454|0.753|0.136|-0.467|0.411|0.336|-0.052|-0.987|-0.057|0.746|0.815|-0.798|-0.374|0.151|-0.825|0.296|-0.256|0.515|0.234|-0.852|0.186|0.838|-0.207|0.579|0.045|-0.787|-0.534</v>
+        <v>0.33|-0.901|-0.072|0.178|0.204|-0.311|0.815|0.04|0.416|0.148|-0.81|-0.106|0.22|-0.643|0.863|-0.761|0.519|0.439|-0.854|0.05|text|text|text3|-0.695|0.857|0.712|0.895|0.593|-0.909|0.609|0.498|text|0.077|-0.094|-0.514|-0.85|-0.618|0.786|0.451|-0.858|-0.946|text|||text|0.858|0.428|-0.128|-0.67|-0.859|-0.657|0.574|-0.813|text2|-0.868|-0.044|-0.62|0.582|0.626|-0.085|0.163|-0.192|0.174|-0.1|0.965|0.466|-0.266|-0.713|-0.145|0.101|0.098|-0.139|-0.271|0.542|-0.859|-0.508|0.172|0.971|0.294|0.882|-0.053|-0.641|-0.525|-0.35|-0.636</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12">
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="str">
+        <f ca="1">_xll.acq_join(J2:J18, "|")</f>
+        <v>-0.514|-0.85|-0.618|0.786|0.451|-0.858|-0.946|text|||text|0.858|0.428|-0.128|-0.67|-0.859|-0.657</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12">
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="str">
+        <f ca="1">_xll.acq_join(H7:L7, "|")</f>
+        <v>-0.311|text3|-0.858|-0.62|0.542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added async handles for long running tasks
</commit_message>
<xml_diff>
--- a/Distribution/Examples/ACQ.Stats.xlsx
+++ b/Distribution/Examples/ACQ.Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDDD7A4-C8DA-48D0-9515-CF681486F93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114E721B-FDD4-4CFA-9615-49920AC157C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5595" yWindow="615" windowWidth="24000" windowHeight="13830" tabRatio="900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="3" r:id="rId1"/>
@@ -576,10 +576,10 @@
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1"/>
     <xf numFmtId="169" fontId="5" fillId="4" borderId="2" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -1449,8 +1449,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:N56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1502,18 +1502,18 @@
       </c>
       <c r="C4" s="6" t="str">
         <f>_xll.acq_version()</f>
-        <v>1.5.8041.39857</v>
+        <v>1.5.8041.40654</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="13">
         <f ca="1">TODAY()</f>
-        <v>44567</v>
+        <v>44578</v>
       </c>
       <c r="J4" s="14" t="str">
         <f ca="1">_xll.acq_tostring(H4)</f>
-        <v>44567</v>
+        <v>44578</v>
       </c>
     </row>
     <row r="5" spans="2:10">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="H13" t="str">
         <f ca="1">_xll.acq_join(H3:H10)</f>
-        <v>3.14159265358979,44567,True,,,,,</v>
+        <v>3.14159265358979,44578,True,,,,,</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" thickBot="1">
@@ -1660,7 +1660,7 @@
       </c>
       <c r="H14" t="str">
         <f ca="1">_xll.acq_join(J3:J10, "|")</f>
-        <v>3.14159265358979|44567|TRUE|||||</v>
+        <v>3.14159265358979|44578|TRUE|||||</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1">
@@ -2208,7 +2208,7 @@
   <dimension ref="A3:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2582,8 +2582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F123368-5BB9-4931-95EC-690D8D570C5B}">
   <dimension ref="A1:Q806"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2609,12 +2609,12 @@
       <c r="B2" s="5">
         <v>0.95</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
     </row>
     <row r="3" spans="1:17">
       <c r="O3" t="s">
@@ -2672,10 +2672,10 @@
         <f>_xll.acq_binomtest(E5,F5,$B$2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="28">
         <v>0.5</v>
       </c>
-      <c r="K5" s="29">
+      <c r="K5" s="28">
         <v>0</v>
       </c>
       <c r="L5">
@@ -2713,10 +2713,10 @@
         <f>_xll.acq_binomtest(E6,F6,$B$2,FALSE)</f>
         <v>0.2775327998628892</v>
       </c>
-      <c r="J6" s="29">
+      <c r="J6" s="28">
         <v>0.75</v>
       </c>
-      <c r="K6" s="29">
+      <c r="K6" s="28">
         <v>0</v>
       </c>
       <c r="L6">
@@ -2746,10 +2746,10 @@
         <f>_xll.acq_binomtest(E7,F7,$B$2,FALSE)</f>
         <v>0.40415002679523848</v>
       </c>
-      <c r="J7" s="29">
+      <c r="J7" s="28">
         <v>1</v>
       </c>
-      <c r="K7" s="29">
+      <c r="K7" s="28">
         <v>0</v>
       </c>
       <c r="L7">
@@ -2779,10 +2779,10 @@
         <f>_xll.acq_binomtest(E8,F8,$B$2,FALSE)</f>
         <v>0.50983752846335817</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J8" s="28">
         <v>1.25</v>
       </c>
-      <c r="K8" s="29">
+      <c r="K8" s="28">
         <v>0</v>
       </c>
       <c r="L8">
@@ -2805,10 +2805,10 @@
         <f>_xll.acq_binomtest(E9,F9,$B$2,FALSE)</f>
         <v>0.60322185253885463</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9" s="28">
         <v>1.5</v>
       </c>
-      <c r="K9" s="29">
+      <c r="K9" s="28">
         <v>0</v>
       </c>
       <c r="L9">
@@ -2831,10 +2831,10 @@
         <f>_xll.acq_binomtest(E10,F10,$B$2,FALSE)</f>
         <v>0.68732623026634165</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="28">
         <v>1.75</v>
       </c>
-      <c r="K10" s="29">
+      <c r="K10" s="28">
         <v>0</v>
       </c>
       <c r="L10">
@@ -2857,10 +2857,10 @@
         <f>_xll.acq_binomtest(E11,F11,$B$2,FALSE)</f>
         <v>0.76340690948743595</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="28">
         <v>1.75</v>
       </c>
-      <c r="K11" s="29">
+      <c r="K11" s="28">
         <v>1</v>
       </c>
       <c r="L11">
@@ -2883,10 +2883,10 @@
         <f>_xll.acq_binomtest(E12,F12,$B$2,FALSE)</f>
         <v>0.8318196702937638</v>
       </c>
-      <c r="J12" s="29">
+      <c r="J12" s="28">
         <v>2</v>
       </c>
-      <c r="K12" s="29">
+      <c r="K12" s="28">
         <v>0</v>
       </c>
       <c r="L12">
@@ -2909,10 +2909,10 @@
         <f>_xll.acq_binomtest(E13,F13,$B$2,FALSE)</f>
         <v>0.89220873259369882</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J13" s="28">
         <v>2.25</v>
       </c>
-      <c r="K13" s="29">
+      <c r="K13" s="28">
         <v>1</v>
       </c>
       <c r="L13">
@@ -2935,10 +2935,10 @@
         <f>_xll.acq_binomtest(E14,F14,$B$2,FALSE)</f>
         <v>0.94331784854562473</v>
       </c>
-      <c r="J14" s="29">
+      <c r="J14" s="28">
         <v>2.5</v>
       </c>
-      <c r="K14" s="29">
+      <c r="K14" s="28">
         <v>0</v>
       </c>
       <c r="L14">
@@ -2961,10 +2961,10 @@
         <f>_xll.acq_binomtest(E15,F15,$B$2,FALSE)</f>
         <v>0.98212378690492708</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="28">
         <v>2.75</v>
       </c>
-      <c r="K15" s="29">
+      <c r="K15" s="28">
         <v>1</v>
       </c>
       <c r="L15">
@@ -2987,10 +2987,10 @@
         <f>_xll.acq_binomtest(E16,F16,$B$2,FALSE)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="J16" s="29">
+      <c r="J16" s="28">
         <v>3</v>
       </c>
-      <c r="K16" s="29">
+      <c r="K16" s="28">
         <v>0</v>
       </c>
       <c r="L16">
@@ -3013,10 +3013,10 @@
         <f>_xll.acq_binomtest(E17,F17,$B$2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J17" s="29">
+      <c r="J17" s="28">
         <v>3.25</v>
       </c>
-      <c r="K17" s="29">
+      <c r="K17" s="28">
         <v>1</v>
       </c>
       <c r="L17">
@@ -3039,10 +3039,10 @@
         <f>_xll.acq_binomtest(E18,F18,$B$2,FALSE)</f>
         <v>0.99823256793585935</v>
       </c>
-      <c r="J18" s="29">
+      <c r="J18" s="28">
         <v>3.5</v>
       </c>
-      <c r="K18" s="29">
+      <c r="K18" s="28">
         <v>0</v>
       </c>
       <c r="L18">
@@ -3065,10 +3065,10 @@
         <f>_xll.acq_binomtest(E19,F19,$B$2,FALSE)</f>
         <v>5.4486196178705315E-2</v>
       </c>
-      <c r="J19" s="29">
+      <c r="J19" s="28">
         <v>4</v>
       </c>
-      <c r="K19" s="29">
+      <c r="K19" s="28">
         <v>1</v>
       </c>
       <c r="L19">
@@ -3077,10 +3077,10 @@
       </c>
     </row>
     <row r="20" spans="5:12">
-      <c r="J20" s="29">
+      <c r="J20" s="28">
         <v>4.25</v>
       </c>
-      <c r="K20" s="29">
+      <c r="K20" s="28">
         <v>1</v>
       </c>
       <c r="L20">
@@ -3089,10 +3089,10 @@
       </c>
     </row>
     <row r="21" spans="5:12">
-      <c r="J21" s="29">
+      <c r="J21" s="28">
         <v>4.5</v>
       </c>
-      <c r="K21" s="29">
+      <c r="K21" s="28">
         <v>1</v>
       </c>
       <c r="L21">
@@ -3101,10 +3101,10 @@
       </c>
     </row>
     <row r="22" spans="5:12">
-      <c r="J22" s="29">
+      <c r="J22" s="28">
         <v>4.75</v>
       </c>
-      <c r="K22" s="29">
+      <c r="K22" s="28">
         <v>1</v>
       </c>
       <c r="L22">
@@ -3113,10 +3113,10 @@
       </c>
     </row>
     <row r="23" spans="5:12">
-      <c r="J23" s="29">
+      <c r="J23" s="28">
         <v>5</v>
       </c>
-      <c r="K23" s="29">
+      <c r="K23" s="28">
         <v>1</v>
       </c>
       <c r="L23">
@@ -3125,10 +3125,10 @@
       </c>
     </row>
     <row r="24" spans="5:12">
-      <c r="J24" s="29">
+      <c r="J24" s="28">
         <v>5.5</v>
       </c>
-      <c r="K24" s="29">
+      <c r="K24" s="28">
         <v>1</v>
       </c>
       <c r="L24">
@@ -5499,8 +5499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30B9D5F-797C-49CC-9435-B3BF433B0ECB}">
   <dimension ref="B1:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5525,11 +5525,11 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">_xll.acq_min(H2:L18)</f>
-        <v>-0.98899999999999999</v>
+        <v>-0.92400000000000004</v>
       </c>
       <c r="D2" s="6">
         <f t="array" aca="1" ref="D2" ca="1">MIN(IF(ISNUMBER(H2:L18), H2:L18))</f>
-        <v>-0.98899999999999999</v>
+        <v>-0.92400000000000004</v>
       </c>
       <c r="E2">
         <f ca="1">C2-D2</f>
@@ -5537,23 +5537,23 @@
       </c>
       <c r="H2" s="5">
         <f ca="1">RANDBETWEEN(-1000,1000)/1000</f>
-        <v>-0.59299999999999997</v>
+        <v>-0.214</v>
       </c>
       <c r="I2" s="5">
         <f t="shared" ref="I2:L18" ca="1" si="0">RANDBETWEEN(-1000,1000)/1000</f>
-        <v>-0.73499999999999999</v>
+        <v>-0.88100000000000001</v>
       </c>
       <c r="J2" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.96499999999999997</v>
+        <v>-0.497</v>
       </c>
       <c r="K2" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.35299999999999998</v>
+        <v>-0.38500000000000001</v>
       </c>
       <c r="L2" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33300000000000002</v>
+        <v>-0.61899999999999999</v>
       </c>
     </row>
     <row r="3" spans="2:12">
@@ -5562,7 +5562,7 @@
       </c>
       <c r="C3" s="6">
         <f ca="1">_xll.acq_absmin(H2:L18)</f>
-        <v>1.0999999999999999E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="D3" s="6">
         <f t="array" aca="1" ref="D3" ca="1">MIN(ABS(IF(ISNUMBER(H2:L18), H2:L18)))</f>
@@ -5570,27 +5570,27 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E11" ca="1" si="1">C3-D3</f>
-        <v>1.0999999999999999E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" ref="H3:H18" ca="1" si="2">RANDBETWEEN(-1000,1000)/1000</f>
-        <v>0.41399999999999998</v>
+        <v>-0.09</v>
       </c>
       <c r="I3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54300000000000004</v>
+        <v>-0.57799999999999996</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1999999999999998E-2</v>
+        <v>-0.108</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41599999999999998</v>
+        <v>-0.76200000000000001</v>
       </c>
       <c r="L3" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47499999999999998</v>
+        <v>-0.23300000000000001</v>
       </c>
     </row>
     <row r="4" spans="2:12">
@@ -5599,11 +5599,11 @@
       </c>
       <c r="C4" s="6">
         <f ca="1">_xll.acq_max(H2:L18)</f>
-        <v>0.93200000000000005</v>
+        <v>0.94399999999999995</v>
       </c>
       <c r="D4" s="6">
         <f t="array" aca="1" ref="D4" ca="1">MAX(IF(ISNUMBER(H2:L18), H2:L18))</f>
-        <v>0.93200000000000005</v>
+        <v>0.94399999999999995</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
@@ -5611,22 +5611,22 @@
       </c>
       <c r="H4" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.79100000000000004</v>
+        <v>0.40300000000000002</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.55500000000000005</v>
+        <v>0.58299999999999996</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.80300000000000005</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>55</v>
       </c>
       <c r="L4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88300000000000001</v>
+        <v>-0.30199999999999999</v>
       </c>
     </row>
     <row r="5" spans="2:12">
@@ -5635,11 +5635,11 @@
       </c>
       <c r="C5" s="6">
         <f ca="1">_xll.acq_absmax(H2:L18)</f>
-        <v>0.98899999999999999</v>
+        <v>0.94399999999999995</v>
       </c>
       <c r="D5" s="6">
         <f t="array" aca="1" ref="D5" ca="1">MAX(ABS(IF(ISNUMBER(H2:L18), H2:L18)))</f>
-        <v>0.98899999999999999</v>
+        <v>0.94399999999999995</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
@@ -5647,22 +5647,22 @@
       </c>
       <c r="H5" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.93200000000000005</v>
+        <v>-0.71699999999999997</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>48</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79400000000000004</v>
+        <v>0.83199999999999996</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.13600000000000001</v>
+        <v>0.19400000000000001</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26900000000000002</v>
+        <v>0.54800000000000004</v>
       </c>
     </row>
     <row r="6" spans="2:12">
@@ -5671,11 +5671,11 @@
       </c>
       <c r="C6" s="6">
         <f ca="1">_xll.acq_sum(H2:L18)</f>
-        <v>4.6390000000000002</v>
+        <v>-7.5129999999999999</v>
       </c>
       <c r="D6" s="6">
         <f t="array" aca="1" ref="D6" ca="1">SUM(IF(ISNUMBER(H2:L18), H2:L18))</f>
-        <v>4.6390000000000002</v>
+        <v>-7.5129999999999999</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
@@ -5683,22 +5683,22 @@
       </c>
       <c r="H6" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.98099999999999998</v>
+        <v>0.19400000000000001</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>48</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.97</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.626</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.32900000000000001</v>
+        <v>0.50900000000000001</v>
       </c>
     </row>
     <row r="7" spans="2:12">
@@ -5707,7 +5707,7 @@
       </c>
       <c r="C7" s="6">
         <f ca="1">_xll.acq_count_unique(H2:L18)</f>
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D7" s="6">
         <f t="array" aca="1" ref="D7" ca="1">COUNT(H2:L18)</f>
@@ -5715,26 +5715,26 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.29599999999999999</v>
+        <v>0.83099999999999996</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>56</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53</v>
+        <v>0.184</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.82699999999999996</v>
+        <v>-4.2000000000000003E-2</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.84499999999999997</v>
+        <v>1.4E-2</v>
       </c>
     </row>
     <row r="8" spans="2:12">
@@ -5743,11 +5743,11 @@
       </c>
       <c r="C8" s="6">
         <f ca="1">_xll.acq_mean(H2:L18)</f>
-        <v>6.1039473684210532E-2</v>
+        <v>-9.8855263157894738E-2</v>
       </c>
       <c r="D8" s="6">
         <f t="array" aca="1" ref="D8" ca="1">AVERAGE(IF(ISNUMBER(H2:L18), H2:L18))</f>
-        <v>6.1039473684210532E-2</v>
+        <v>-9.8855263157894738E-2</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
@@ -5755,23 +5755,23 @@
       </c>
       <c r="H8" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.51100000000000001</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.59199999999999997</v>
+        <v>-0.14299999999999999</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.54800000000000004</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.88</v>
+        <v>-0.19500000000000001</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.52800000000000002</v>
+        <v>-0.6</v>
       </c>
     </row>
     <row r="9" spans="2:12">
@@ -5780,11 +5780,11 @@
       </c>
       <c r="C9" s="6">
         <f ca="1">_xll.acq_stdev(H2:L18)</f>
-        <v>0.59495600825135464</v>
+        <v>0.56395280426521188</v>
       </c>
       <c r="D9" s="6">
         <f t="array" aca="1" ref="D9" ca="1">_xlfn.STDEV.S(IF(ISNUMBER(H2:L18), H2:L18))</f>
-        <v>0.59495600825135464</v>
+        <v>0.56395280426521199</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
@@ -5792,22 +5792,22 @@
       </c>
       <c r="H9" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.51</v>
+        <v>-0.67900000000000005</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86</v>
+        <v>0.93300000000000005</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>48</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.51100000000000001</v>
+        <v>-0.82</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53100000000000003</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="10" spans="2:12">
@@ -5816,11 +5816,11 @@
       </c>
       <c r="C10" s="6">
         <f ca="1">_xll.acq_sumofsquares(H2:L18)</f>
-        <v>26.831111000000007</v>
+        <v>24.59590699999999</v>
       </c>
       <c r="D10" s="6">
         <f t="array" aca="1" ref="D10" ca="1">SUM(IF(ISNUMBER(H2:L18), H2:L18^2))</f>
-        <v>26.831111000000003</v>
+        <v>24.595907</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
@@ -5828,11 +5828,11 @@
       </c>
       <c r="H10" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.92800000000000005</v>
+        <v>-0.80400000000000005</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8000000000000004E-2</v>
+        <v>-0.48599999999999999</v>
       </c>
       <c r="J10" s="5" t="e">
         <f>1/0</f>
@@ -5840,11 +5840,11 @@
       </c>
       <c r="K10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.28000000000000003</v>
+        <v>-0.438</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.34100000000000003</v>
+        <v>-0.71199999999999997</v>
       </c>
     </row>
     <row r="11" spans="2:12">
@@ -5865,11 +5865,11 @@
       </c>
       <c r="H11" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-5.7000000000000002E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.874</v>
+        <v>-0.29399999999999998</v>
       </c>
       <c r="J11" s="5" t="e">
         <f>SQRT(-1)</f>
@@ -5877,163 +5877,163 @@
       </c>
       <c r="K11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.14199999999999999</v>
+        <v>-0.11799999999999999</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.109</v>
+        <v>0.69599999999999995</v>
       </c>
     </row>
     <row r="12" spans="2:12">
       <c r="H12" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.89</v>
+        <v>-0.91500000000000004</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28599999999999998</v>
+        <v>0.46800000000000003</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>48</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27300000000000002</v>
+        <v>-0.872</v>
       </c>
       <c r="L12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.5000000000000006E-2</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="13" spans="2:12">
       <c r="H13" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.77</v>
+        <v>0.91100000000000003</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.746</v>
+        <v>-0.79600000000000004</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.42399999999999999</v>
+        <v>0.58299999999999996</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63</v>
+        <v>-5.8999999999999997E-2</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26900000000000002</v>
+        <v>-0.30299999999999999</v>
       </c>
     </row>
     <row r="14" spans="2:12">
       <c r="H14" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.52900000000000003</v>
+        <v>0.30199999999999999</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.98899999999999999</v>
+        <v>-0.92400000000000004</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.0999999999999999E-2</v>
+        <v>0.94399999999999995</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.67400000000000004</v>
+        <v>0.48199999999999998</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.90900000000000003</v>
+        <v>-0.84199999999999997</v>
       </c>
     </row>
     <row r="15" spans="2:12">
       <c r="H15" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.23400000000000001</v>
+        <v>-0.90200000000000002</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91200000000000003</v>
+        <v>0.32300000000000001</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5E-2</v>
+        <v>-0.48</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.89400000000000002</v>
+        <v>-0.54</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.498</v>
+        <v>-0.54100000000000004</v>
       </c>
     </row>
     <row r="16" spans="2:12">
       <c r="H16" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.68700000000000006</v>
+        <v>-0.51400000000000001</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>48</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.29299999999999998</v>
+        <v>-0.23599999999999999</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6000000000000003E-2</v>
+        <v>-0.61299999999999999</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8000000000000003E-2</v>
+        <v>-0.57799999999999996</v>
       </c>
     </row>
     <row r="17" spans="2:12">
       <c r="H17" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>2.5999999999999999E-2</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="I17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.438</v>
+        <v>-0.14799999999999999</v>
       </c>
       <c r="J17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54700000000000004</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.309</v>
+        <v>0.76800000000000002</v>
       </c>
       <c r="L17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.65900000000000003</v>
+        <v>-0.45400000000000001</v>
       </c>
     </row>
     <row r="18" spans="2:12">
       <c r="H18" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.38400000000000001</v>
+        <v>-0.13800000000000001</v>
       </c>
       <c r="I18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69499999999999995</v>
+        <v>3.9E-2</v>
       </c>
       <c r="J18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27300000000000002</v>
+        <v>-0.26700000000000002</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26500000000000001</v>
+        <v>-0.73499999999999999</v>
       </c>
       <c r="L18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.90700000000000003</v>
+        <v>-0.872</v>
       </c>
     </row>
     <row r="25" spans="2:12">
@@ -6042,7 +6042,7 @@
       </c>
       <c r="C25" t="str">
         <f ca="1">_xll.acq_join(H2:L18, "|")</f>
-        <v>-0.593|0.414|0.791|0.932|-0.981|-0.296|0.511|0.51|0.928|-0.057|0.89|0.77|-0.529|-0.234|-0.687|0.026|0.384|-0.735|0.543|-0.555|text|text|text3|-0.592|0.86|0.098|0.874|0.286|0.746|-0.989|0.912|text|-0.438|0.695|-0.965|0.052|0.803|0.794|-0.97|0.53|-0.548|text|||text|-0.424|-0.011|0.055|-0.293|0.547|0.273|-0.353|0.416|text2|-0.136|0.626|-0.827|-0.88|-0.511|-0.28|-0.142|0.273|0.63|-0.674|0.894|0.066|0.309|0.265|0.333|0.475|0.883|0.269|-0.329|-0.845|-0.528|0.531|-0.341|0.109|-0.085|0.269|-0.909|0.498|0.058|-0.659|0.907</v>
+        <v>-0.214|-0.09|0.403|-0.717|0.194|0.831|0.177|-0.679|-0.804|0.079|-0.915|0.911|0.302|-0.902|-0.514|0.885|-0.138|-0.881|-0.578|0.583|text|text|text3|-0.143|0.933|-0.486|-0.294|0.468|-0.796|-0.924|0.323|text|-0.148|0.039|-0.497|-0.108|0.396|0.832|0.209|0.184|0.712|text|||text|0.583|0.944|-0.48|-0.236|0.765|-0.267|-0.385|-0.762|text2|0.194|0.808|-0.042|-0.195|-0.82|-0.438|-0.118|-0.872|-0.059|0.482|-0.54|-0.613|0.768|-0.735|-0.619|-0.233|-0.302|0.548|0.509|0.014|-0.6|0.001|-0.712|0.696|0.16|-0.303|-0.842|-0.541|-0.578|-0.454|-0.872</v>
       </c>
     </row>
     <row r="26" spans="2:12">
@@ -6051,7 +6051,7 @@
       </c>
       <c r="C26" t="str">
         <f ca="1">_xll.acq_join(J2:J18, "|")</f>
-        <v>-0.965|0.052|0.803|0.794|-0.97|0.53|-0.548|text|||text|-0.424|-0.011|0.055|-0.293|0.547|0.273</v>
+        <v>-0.497|-0.108|0.396|0.832|0.209|0.184|0.712|text|||text|0.583|0.944|-0.48|-0.236|0.765|-0.267</v>
       </c>
     </row>
     <row r="27" spans="2:12">
@@ -6060,7 +6060,7 @@
       </c>
       <c r="C27" t="str">
         <f ca="1">_xll.acq_join(H7:L7, "|")</f>
-        <v>-0.296|text3|0.53|-0.827|-0.845</v>
+        <v>0.831|text3|0.184|-0.042|0.014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>